<commit_message>
color spectrum working correctly
</commit_message>
<xml_diff>
--- a/All_Lows.xlsx
+++ b/All_Lows.xlsx
@@ -67,7 +67,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -76,104 +76,194 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF4D4D"/>
-        <bgColor rgb="00FF4D4D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00E60000"/>
-        <bgColor rgb="00E60000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00CC0000"/>
-        <bgColor rgb="00CC0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00E6E600"/>
-        <bgColor rgb="00E6E600"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF9999"/>
-        <bgColor rgb="00FF9999"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="00FF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF6666"/>
-        <bgColor rgb="00FF6666"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00B20000"/>
-        <bgColor rgb="00B20000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0085FF85"/>
-        <bgColor rgb="0085FF85"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0075FF75"/>
-        <bgColor rgb="0075FF75"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="005CE65C"/>
-        <bgColor rgb="005CE65C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0052CC52"/>
-        <bgColor rgb="0052CC52"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0047B247"/>
-        <bgColor rgb="0047B247"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00990000"/>
-        <bgColor rgb="00990000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF8080"/>
-        <bgColor rgb="00FF8080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF1919"/>
-        <bgColor rgb="00FF1919"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF3333"/>
-        <bgColor rgb="00FF3333"/>
+        <fgColor rgb="00FF2000"/>
+        <bgColor rgb="00FF2000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF4000"/>
+        <bgColor rgb="00FF4000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF5800"/>
+        <bgColor rgb="00FF5800"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFEF00"/>
+        <bgColor rgb="00FFEF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E7FF00"/>
+        <bgColor rgb="00E7FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF4800"/>
+        <bgColor rgb="00FF4800"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF1000"/>
+        <bgColor rgb="00FF1000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF1800"/>
+        <bgColor rgb="00FF1800"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0068FF00"/>
+        <bgColor rgb="0068FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DFFF00"/>
+        <bgColor rgb="00DFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0060FF00"/>
+        <bgColor rgb="0060FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0058FF00"/>
+        <bgColor rgb="0058FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0040FF00"/>
+        <bgColor rgb="0040FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0020FF00"/>
+        <bgColor rgb="0020FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0038FF00"/>
+        <bgColor rgb="0038FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0010FF00"/>
+        <bgColor rgb="0010FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0008FF00"/>
+        <bgColor rgb="0008FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0018FF00"/>
+        <bgColor rgb="0018FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0028FF00"/>
+        <bgColor rgb="0028FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000FF00"/>
+        <bgColor rgb="0000FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0030FF00"/>
+        <bgColor rgb="0030FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0050FF00"/>
+        <bgColor rgb="0050FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0048FF00"/>
+        <bgColor rgb="0048FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F7FF00"/>
+        <bgColor rgb="00F7FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFDF00"/>
+        <bgColor rgb="00FFDF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFE700"/>
+        <bgColor rgb="00FFE700"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF5000"/>
+        <bgColor rgb="00FF5000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EFFF00"/>
+        <bgColor rgb="00EFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF2800"/>
+        <bgColor rgb="00FF2800"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF3000"/>
+        <bgColor rgb="00FF3000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF700"/>
+        <bgColor rgb="00FFF700"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF3800"/>
+        <bgColor rgb="00FF3800"/>
       </patternFill>
     </fill>
   </fills>
@@ -204,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="33">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
@@ -255,6 +345,51 @@
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="18" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="19" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="20" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="21" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="22" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="23" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="24" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="25" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="26" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="27" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="28" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="29" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="30" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="31" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="32" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="33" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -550,7 +685,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -604,40 +739,40 @@
       <c t="n" r="A2">
         <v>1990</v>
       </c>
-      <c s="1" t="n" r="B2">
+      <c t="n" s="1" r="B2">
         <v>25.36</v>
       </c>
-      <c s="2" t="n" r="C2">
+      <c t="n" s="2" r="C2">
         <v>21.99</v>
       </c>
-      <c s="3" t="n" r="D2">
+      <c t="n" s="3" r="D2">
         <v>19.73</v>
       </c>
-      <c s="3" t="n" r="E2">
+      <c t="n" s="3" r="E2">
         <v>19.52</v>
       </c>
-      <c s="4" t="n" r="F2">
+      <c t="n" s="4" r="F2">
         <v>17.37</v>
       </c>
-      <c s="4" t="n" r="G2">
+      <c t="n" s="5" r="G2">
         <v>15.5</v>
       </c>
-      <c s="2" t="n" r="H2">
+      <c t="n" s="6" r="H2">
         <v>21.11</v>
       </c>
-      <c s="5" t="n" r="I2">
+      <c t="n" s="7" r="I2">
         <v>29.9</v>
       </c>
-      <c s="5" t="n" r="J2">
+      <c t="n" s="7" r="J2">
         <v>29.11</v>
       </c>
-      <c s="5" t="n" r="K2">
+      <c t="n" s="7" r="K2">
         <v>30.04</v>
       </c>
-      <c s="6" t="n" r="L2">
+      <c t="n" s="2" r="L2">
         <v>22.16</v>
       </c>
-      <c s="7" t="n" r="M2">
+      <c t="n" s="8" r="M2">
         <v>26.38</v>
       </c>
     </row>
@@ -645,40 +780,40 @@
       <c t="n" r="A3">
         <v>1991</v>
       </c>
-      <c s="8" t="n" r="B3">
+      <c t="n" s="6" r="B3">
         <v>20.91</v>
       </c>
-      <c s="3" t="n" r="C3">
+      <c t="n" s="3" r="C3">
         <v>19.57</v>
       </c>
-      <c s="9" t="n" r="D3">
+      <c t="n" s="9" r="D3">
         <v>14.9</v>
       </c>
-      <c s="4" t="n" r="E3">
+      <c t="n" s="5" r="E3">
         <v>15.47</v>
       </c>
-      <c s="4" t="n" r="F3">
+      <c t="n" s="10" r="F3">
         <v>15.23</v>
       </c>
-      <c s="4" t="n" r="G3">
+      <c t="n" s="5" r="G3">
         <v>15.5</v>
       </c>
-      <c s="4" t="n" r="H3">
+      <c t="n" s="10" r="H3">
         <v>15.18</v>
       </c>
-      <c s="9" t="n" r="I3">
+      <c t="n" s="11" r="I3">
         <v>14.41</v>
       </c>
-      <c s="9" t="n" r="J3">
+      <c t="n" s="11" r="J3">
         <v>14.46</v>
       </c>
-      <c s="9" t="n" r="K3">
+      <c t="n" s="9" r="K3">
         <v>14.81</v>
       </c>
-      <c s="9" t="n" r="L3">
+      <c t="n" s="12" r="L3">
         <v>13.95</v>
       </c>
-      <c s="4" t="n" r="M3">
+      <c t="n" s="5" r="M3">
         <v>15.44</v>
       </c>
     </row>
@@ -686,40 +821,40 @@
       <c t="n" r="A4">
         <v>1992</v>
       </c>
-      <c s="9" t="n" r="B4">
+      <c t="n" s="12" r="B4">
         <v>14.12</v>
       </c>
-      <c s="9" t="n" r="C4">
+      <c t="n" s="12" r="C4">
         <v>14.12</v>
       </c>
-      <c s="4" t="n" r="D4">
+      <c t="n" s="10" r="D4">
         <v>15.34</v>
       </c>
-      <c s="9" t="n" r="E4">
+      <c t="n" s="9" r="E4">
         <v>14.83</v>
       </c>
-      <c s="10" t="n" r="F4">
+      <c t="n" s="13" r="F4">
         <v>12.77</v>
       </c>
-      <c s="10" t="n" r="G4">
+      <c t="n" s="13" r="G4">
         <v>12.73</v>
       </c>
-      <c s="11" t="n" r="H4">
+      <c t="n" s="14" r="H4">
         <v>11.36</v>
       </c>
-      <c s="10" t="n" r="I4">
+      <c t="n" s="15" r="I4">
         <v>12.34</v>
       </c>
-      <c s="12" t="n" r="J4">
+      <c t="n" s="16" r="J4">
         <v>10.69</v>
       </c>
-      <c s="4" t="n" r="K4">
+      <c t="n" s="10" r="K4">
         <v>15.03</v>
       </c>
-      <c s="11" t="n" r="L4">
+      <c t="n" s="14" r="L4">
         <v>11.38</v>
       </c>
-      <c s="12" t="n" r="M4">
+      <c t="n" s="17" r="M4">
         <v>10.29</v>
       </c>
     </row>
@@ -727,40 +862,40 @@
       <c t="n" r="A5">
         <v>1993</v>
       </c>
-      <c s="12" t="n" r="B5">
+      <c t="n" s="18" r="B5">
         <v>10.98</v>
       </c>
-      <c s="11" t="n" r="C5">
+      <c t="n" s="19" r="C5">
         <v>11.69</v>
       </c>
-      <c s="12" t="n" r="D5">
+      <c t="n" s="16" r="D5">
         <v>10.66</v>
       </c>
-      <c s="12" t="n" r="E5">
+      <c t="n" s="16" r="E5">
         <v>10.71</v>
       </c>
-      <c s="11" t="n" r="F5">
+      <c t="n" s="14" r="F5">
         <v>11.25</v>
       </c>
-      <c s="12" t="n" r="G5">
+      <c t="n" s="18" r="G5">
         <v>10.86</v>
       </c>
-      <c s="13" t="n" r="H5">
+      <c t="n" s="20" r="H5">
         <v>9.109999999999999</v>
       </c>
-      <c s="12" t="n" r="I5">
+      <c t="n" s="17" r="I5">
         <v>10.34</v>
       </c>
-      <c s="12" t="n" r="J5">
+      <c t="n" s="16" r="J5">
         <v>10.75</v>
       </c>
-      <c s="13" t="n" r="K5">
+      <c t="n" s="17" r="K5">
         <v>10</v>
       </c>
-      <c s="11" t="n" r="L5">
+      <c t="n" s="14" r="L5">
         <v>11.49</v>
       </c>
-      <c s="13" t="n" r="M5">
+      <c t="n" s="20" r="M5">
         <v>8.890000000000001</v>
       </c>
     </row>
@@ -768,40 +903,40 @@
       <c t="n" r="A6">
         <v>1994</v>
       </c>
-      <c s="13" t="n" r="B6">
+      <c t="n" s="20" r="B6">
         <v>9.59</v>
       </c>
-      <c s="12" t="n" r="C6">
+      <c t="n" s="17" r="C6">
         <v>10.21</v>
       </c>
-      <c s="11" t="n" r="D6">
+      <c t="n" s="19" r="D6">
         <v>11.58</v>
       </c>
-      <c s="9" t="n" r="E6">
+      <c t="n" s="13" r="E6">
         <v>13.05</v>
       </c>
-      <c s="11" t="n" r="F6">
+      <c t="n" s="14" r="F6">
         <v>11.44</v>
       </c>
-      <c s="12" t="n" r="G6">
+      <c t="n" s="16" r="G6">
         <v>10.48</v>
       </c>
-      <c s="12" t="n" r="H6">
+      <c t="n" s="18" r="H6">
         <v>10.96</v>
       </c>
-      <c s="12" t="n" r="I6">
+      <c t="n" s="16" r="I6">
         <v>10.75</v>
       </c>
-      <c s="11" t="n" r="J6">
+      <c t="n" s="14" r="J6">
         <v>11.17</v>
       </c>
-      <c s="10" t="n" r="K6">
+      <c t="n" s="13" r="K6">
         <v>12.75</v>
       </c>
-      <c s="9" t="n" r="L6">
+      <c t="n" s="11" r="L6">
         <v>14.32</v>
       </c>
-      <c s="11" t="n" r="M6">
+      <c t="n" s="14" r="M6">
         <v>11.36</v>
       </c>
     </row>
@@ -809,40 +944,40 @@
       <c t="n" r="A7">
         <v>1995</v>
       </c>
-      <c s="12" t="n" r="B7">
+      <c t="n" s="16" r="B7">
         <v>10.76</v>
       </c>
-      <c s="12" t="n" r="C7">
+      <c t="n" s="16" r="C7">
         <v>10.51</v>
       </c>
-      <c s="12" t="n" r="D7">
+      <c t="n" s="18" r="D7">
         <v>10.79</v>
       </c>
-      <c s="12" t="n" r="E7">
+      <c t="n" s="18" r="E7">
         <v>10.95</v>
       </c>
-      <c s="12" t="n" r="F7">
+      <c t="n" s="17" r="F7">
         <v>10.08</v>
       </c>
-      <c s="12" t="n" r="G7">
+      <c t="n" s="17" r="G7">
         <v>10.36</v>
       </c>
-      <c s="12" t="n" r="H7">
+      <c t="n" s="16" r="H7">
         <v>10.75</v>
       </c>
-      <c s="11" t="n" r="I7">
+      <c t="n" s="14" r="I7">
         <v>11.36</v>
       </c>
-      <c s="12" t="n" r="J7">
+      <c t="n" s="17" r="J7">
         <v>10.19</v>
       </c>
-      <c s="10" t="n" r="K7">
+      <c t="n" s="21" r="K7">
         <v>12.09</v>
       </c>
-      <c s="12" t="n" r="L7">
+      <c t="n" s="16" r="L7">
         <v>10.57</v>
       </c>
-      <c s="12" t="n" r="M7">
+      <c t="n" s="17" r="M7">
         <v>10.06</v>
       </c>
     </row>
@@ -850,40 +985,40 @@
       <c t="n" r="A8">
         <v>1996</v>
       </c>
-      <c s="11" t="n" r="B8">
+      <c t="n" s="14" r="B8">
         <v>11.23</v>
       </c>
-      <c s="11" t="n" r="C8">
+      <c t="n" s="18" r="C8">
         <v>11.11</v>
       </c>
-      <c s="9" t="n" r="D8">
+      <c t="n" s="9" r="D8">
         <v>14.98</v>
       </c>
-      <c s="9" t="n" r="E8">
+      <c t="n" s="12" r="E8">
         <v>13.99</v>
       </c>
-      <c s="9" t="n" r="F8">
+      <c t="n" s="11" r="F8">
         <v>14.56</v>
       </c>
-      <c s="9" t="n" r="G8">
+      <c t="n" s="22" r="G8">
         <v>13.55</v>
       </c>
-      <c s="9" t="n" r="H8">
+      <c t="n" s="22" r="H8">
         <v>13.75</v>
       </c>
-      <c s="9" t="n" r="I8">
+      <c t="n" s="23" r="I8">
         <v>13.22</v>
       </c>
-      <c s="9" t="n" r="J8">
+      <c t="n" s="11" r="J8">
         <v>14.55</v>
       </c>
-      <c s="9" t="n" r="K8">
+      <c t="n" s="9" r="K8">
         <v>14.63</v>
       </c>
-      <c s="9" t="n" r="L8">
+      <c t="n" s="23" r="L8">
         <v>13.45</v>
       </c>
-      <c s="4" t="n" r="M8">
+      <c t="n" s="24" r="M8">
         <v>16.68</v>
       </c>
     </row>
@@ -891,40 +1026,40 @@
       <c t="n" r="A9">
         <v>1997</v>
       </c>
-      <c s="4" t="n" r="B9">
+      <c t="n" s="24" r="B9">
         <v>16.36</v>
       </c>
-      <c s="14" t="n" r="C9">
+      <c t="n" s="25" r="C9">
         <v>18.71</v>
       </c>
-      <c s="4" t="n" r="D9">
+      <c t="n" s="4" r="D9">
         <v>17.3</v>
       </c>
-      <c s="4" t="n" r="E9">
+      <c t="n" s="4" r="E9">
         <v>17.57</v>
       </c>
-      <c s="4" t="n" r="F9">
+      <c t="n" s="4" r="F9">
         <v>17.28</v>
       </c>
-      <c s="14" t="n" r="G9">
+      <c t="n" s="25" r="G9">
         <v>18.2</v>
       </c>
-      <c s="4" t="n" r="H9">
+      <c t="n" s="26" r="H9">
         <v>17.82</v>
       </c>
-      <c s="3" t="n" r="I9">
+      <c t="n" s="3" r="I9">
         <v>19.33</v>
       </c>
-      <c s="2" t="n" r="J9">
+      <c t="n" s="6" r="J9">
         <v>21.43</v>
       </c>
-      <c s="3" t="n" r="K9">
+      <c t="n" s="3" r="K9">
         <v>19.28</v>
       </c>
-      <c s="7" t="n" r="L9">
+      <c t="n" s="8" r="L9">
         <v>26.42</v>
       </c>
-      <c s="8" t="n" r="M9">
+      <c t="n" s="27" r="M9">
         <v>20.41</v>
       </c>
     </row>
@@ -932,40 +1067,40 @@
       <c t="n" r="A10">
         <v>1998</v>
       </c>
-      <c s="8" t="n" r="B10">
+      <c t="n" s="27" r="B10">
         <v>20.55</v>
       </c>
-      <c s="14" t="n" r="C10">
+      <c t="n" s="25" r="C10">
         <v>18.39</v>
       </c>
-      <c s="4" t="n" r="D10">
+      <c t="n" s="26" r="D10">
         <v>17.58</v>
       </c>
-      <c s="3" t="n" r="E10">
+      <c t="n" s="3" r="E10">
         <v>19.25</v>
       </c>
-      <c s="14" t="n" r="F10">
+      <c t="n" s="25" r="F10">
         <v>18.6</v>
       </c>
-      <c s="14" t="n" r="G10">
+      <c t="n" s="3" r="G10">
         <v>18.93</v>
       </c>
-      <c s="4" t="n" r="H10">
+      <c t="n" s="28" r="H10">
         <v>16.1</v>
       </c>
-      <c s="6" t="n" r="I10">
+      <c t="n" s="2" r="I10">
         <v>22.11</v>
       </c>
-      <c s="5" t="n" r="J10">
+      <c t="n" s="7" r="J10">
         <v>32.44</v>
       </c>
-      <c s="15" t="n" r="K10">
+      <c t="n" s="7" r="K10">
         <v>27.54</v>
       </c>
-      <c s="2" t="n" r="L10">
+      <c t="n" s="6" r="L10">
         <v>21.24</v>
       </c>
-      <c s="8" t="n" r="M10">
+      <c t="n" s="27" r="M10">
         <v>20.08</v>
       </c>
     </row>
@@ -973,40 +1108,40 @@
       <c t="n" r="A11">
         <v>1999</v>
       </c>
-      <c s="2" t="n" r="B11">
+      <c t="n" s="6" r="B11">
         <v>21.38</v>
       </c>
-      <c s="1" t="n" r="C11">
+      <c t="n" s="29" r="C11">
         <v>25.22</v>
       </c>
-      <c s="2" t="n" r="D11">
+      <c t="n" s="2" r="D11">
         <v>22</v>
       </c>
-      <c s="8" t="n" r="E11">
+      <c t="n" s="27" r="E11">
         <v>20.47</v>
       </c>
-      <c s="16" t="n" r="F11">
+      <c t="n" s="30" r="F11">
         <v>23.62</v>
       </c>
-      <c s="8" t="n" r="G11">
+      <c t="n" s="27" r="G11">
         <v>20.67</v>
       </c>
-      <c s="4" t="n" r="H11">
+      <c t="n" s="31" r="H11">
         <v>17.07</v>
       </c>
-      <c s="8" t="n" r="I11">
+      <c t="n" s="27" r="I11">
         <v>20.12</v>
       </c>
-      <c s="8" t="n" r="J11">
+      <c t="n" s="6" r="J11">
         <v>20.87</v>
       </c>
-      <c s="8" t="n" r="K11">
+      <c t="n" s="27" r="K11">
         <v>20.3</v>
       </c>
-      <c s="14" t="n" r="L11">
+      <c t="n" s="25" r="L11">
         <v>18.64</v>
       </c>
-      <c s="14" t="n" r="M11">
+      <c t="n" s="25" r="M11">
         <v>18.69</v>
       </c>
     </row>
@@ -1014,40 +1149,40 @@
       <c t="n" r="A12">
         <v>2000</v>
       </c>
-      <c s="3" t="n" r="B12">
+      <c t="n" s="3" r="B12">
         <v>19.51</v>
       </c>
-      <c s="8" t="n" r="C12">
+      <c t="n" s="27" r="C12">
         <v>20.69</v>
       </c>
-      <c s="3" t="n" r="D12">
+      <c t="n" s="3" r="D12">
         <v>19.19</v>
       </c>
-      <c s="16" t="n" r="E12">
+      <c t="n" s="32" r="E12">
         <v>23.25</v>
       </c>
-      <c s="16" t="n" r="F12">
+      <c t="n" s="32" r="F12">
         <v>23.23</v>
       </c>
-      <c s="3" t="n" r="G12">
+      <c t="n" s="3" r="G12">
         <v>19.39</v>
       </c>
-      <c s="14" t="n" r="H12">
+      <c t="n" s="25" r="H12">
         <v>18.77</v>
       </c>
-      <c s="4" t="n" r="I12">
+      <c t="n" s="28" r="I12">
         <v>16.28</v>
       </c>
-      <c s="4" t="n" r="J12">
+      <c t="n" s="24" r="J12">
         <v>16.47</v>
       </c>
-      <c s="3" t="n" r="K12">
+      <c t="n" s="3" r="K12">
         <v>19.8</v>
       </c>
-      <c s="16" t="n" r="L12">
+      <c t="n" s="30" r="L12">
         <v>23.51</v>
       </c>
-      <c s="6" t="n" r="M12">
+      <c t="n" s="2" r="M12">
         <v>22.38</v>
       </c>
     </row>
@@ -1055,40 +1190,40 @@
       <c t="n" r="A13">
         <v>2001</v>
       </c>
-      <c s="2" t="n" r="B13">
+      <c t="n" s="6" r="B13">
         <v>21.47</v>
       </c>
-      <c s="8" t="n" r="C13">
+      <c t="n" s="27" r="C13">
         <v>20.22</v>
       </c>
-      <c s="17" t="n" r="D13">
+      <c t="n" s="30" r="D13">
         <v>24.12</v>
       </c>
-      <c s="16" t="n" r="E13">
+      <c t="n" s="32" r="E13">
         <v>23.01</v>
       </c>
-      <c s="8" t="n" r="F13">
+      <c t="n" s="27" r="F13">
         <v>20.46</v>
       </c>
-      <c s="14" t="n" r="G13">
+      <c t="n" s="25" r="G13">
         <v>18.83</v>
       </c>
-      <c s="14" t="n" r="H13">
+      <c t="n" s="25" r="H13">
         <v>18.74</v>
       </c>
-      <c s="3" t="n" r="I13">
+      <c t="n" s="3" r="I13">
         <v>19.69</v>
       </c>
-      <c s="17" t="n" r="J13">
+      <c t="n" s="30" r="J13">
         <v>24.19</v>
       </c>
-      <c s="5" t="n" r="K13">
+      <c t="n" s="7" r="K13">
         <v>28.11</v>
       </c>
-      <c s="6" t="n" r="L13">
+      <c t="n" s="32" r="L13">
         <v>22.96</v>
       </c>
-      <c s="2" t="n" r="M13">
+      <c t="n" s="6" r="M13">
         <v>21.12</v>
       </c>
     </row>
@@ -1096,40 +1231,40 @@
       <c t="n" r="A14">
         <v>2002</v>
       </c>
-      <c s="8" t="n" r="B14">
+      <c t="n" s="27" r="B14">
         <v>20.4</v>
       </c>
-      <c s="8" t="n" r="C14">
+      <c t="n" s="27" r="C14">
         <v>20.55</v>
       </c>
-      <c s="4" t="n" r="D14">
+      <c t="n" s="31" r="D14">
         <v>17.02</v>
       </c>
-      <c s="4" t="n" r="E14">
+      <c t="n" s="26" r="E14">
         <v>17.73</v>
       </c>
-      <c s="4" t="n" r="F14">
+      <c t="n" s="26" r="F14">
         <v>17.7</v>
       </c>
-      <c s="3" t="n" r="G14">
+      <c t="n" s="3" r="G14">
         <v>19.43</v>
       </c>
-      <c s="1" t="n" r="H14">
+      <c t="n" s="1" r="H14">
         <v>25.63</v>
       </c>
-      <c s="15" t="n" r="I14">
+      <c t="n" s="7" r="I14">
         <v>27.61</v>
       </c>
-      <c s="5" t="n" r="J14">
+      <c t="n" s="7" r="J14">
         <v>31.93</v>
       </c>
-      <c s="5" t="n" r="K14">
+      <c t="n" s="7" r="K14">
         <v>29.69</v>
       </c>
-      <c s="16" t="n" r="L14">
+      <c t="n" s="32" r="L14">
         <v>23.05</v>
       </c>
-      <c s="1" t="n" r="M14">
+      <c t="n" s="1" r="M14">
         <v>25.87</v>
       </c>
     </row>
@@ -1137,40 +1272,40 @@
       <c t="n" r="A15">
         <v>2003</v>
       </c>
-      <c s="17" t="n" r="B15">
+      <c t="n" s="30" r="B15">
         <v>24.02</v>
       </c>
-      <c s="5" t="n" r="C15">
+      <c t="n" s="7" r="C15">
         <v>29.06</v>
       </c>
-      <c s="15" t="n" r="D15">
+      <c t="n" s="7" r="D15">
         <v>27.58</v>
       </c>
-      <c s="8" t="n" r="E15">
+      <c t="n" s="27" r="E15">
         <v>20.26</v>
       </c>
-      <c s="14" t="n" r="F15">
+      <c t="n" s="25" r="F15">
         <v>18.24</v>
       </c>
-      <c s="14" t="n" r="G15">
+      <c t="n" s="25" r="G15">
         <v>18.87</v>
       </c>
-      <c s="4" t="n" r="H15">
+      <c t="n" s="26" r="H15">
         <v>17.65</v>
       </c>
-      <c s="4" t="n" r="I15">
+      <c t="n" s="26" r="I15">
         <v>17.64</v>
       </c>
-      <c s="4" t="n" r="J15">
+      <c t="n" s="4" r="J15">
         <v>17.52</v>
       </c>
-      <c s="4" t="n" r="K15">
+      <c t="n" s="5" r="K15">
         <v>15.79</v>
       </c>
-      <c s="4" t="n" r="L15">
+      <c t="n" s="5" r="L15">
         <v>15.79</v>
       </c>
-      <c s="9" t="n" r="M15">
+      <c t="n" s="9" r="M15">
         <v>14.66</v>
       </c>
     </row>
@@ -1178,40 +1313,40 @@
       <c t="n" r="A16">
         <v>2004</v>
       </c>
-      <c s="9" t="n" r="B16">
+      <c t="n" s="12" r="B16">
         <v>14.01</v>
       </c>
-      <c s="9" t="n" r="C16">
+      <c t="n" s="22" r="C16">
         <v>13.8</v>
       </c>
-      <c s="9" t="n" r="D16">
+      <c t="n" s="22" r="D16">
         <v>13.83</v>
       </c>
-      <c s="9" t="n" r="E16">
+      <c t="n" s="12" r="E16">
         <v>13.86</v>
       </c>
-      <c s="4" t="n" r="F16">
+      <c t="n" s="10" r="F16">
         <v>15.19</v>
       </c>
-      <c s="9" t="n" r="G16">
+      <c t="n" s="22" r="G16">
         <v>13.75</v>
       </c>
-      <c s="9" t="n" r="H16">
+      <c t="n" s="23" r="H16">
         <v>13.34</v>
       </c>
-      <c s="9" t="n" r="I16">
+      <c t="n" s="9" r="I16">
         <v>14.67</v>
       </c>
-      <c s="9" t="n" r="J16">
+      <c t="n" s="23" r="J16">
         <v>13.16</v>
       </c>
-      <c s="10" t="n" r="K16">
+      <c t="n" s="15" r="K16">
         <v>12.6</v>
       </c>
-      <c s="10" t="n" r="L16">
+      <c t="n" s="15" r="L16">
         <v>12.56</v>
       </c>
-      <c s="11" t="n" r="M16">
+      <c t="n" s="18" r="M16">
         <v>11.14</v>
       </c>
     </row>
@@ -1219,40 +1354,40 @@
       <c t="n" r="A17">
         <v>2005</v>
       </c>
-      <c s="10" t="n" r="B17">
+      <c t="n" s="21" r="B17">
         <v>12.29</v>
       </c>
-      <c s="12" t="n" r="C17">
+      <c t="n" s="18" r="C17">
         <v>10.9</v>
       </c>
-      <c s="11" t="n" r="D17">
+      <c t="n" s="19" r="D17">
         <v>11.66</v>
       </c>
-      <c s="11" t="n" r="E17">
+      <c t="n" s="14" r="E17">
         <v>11.2</v>
       </c>
-      <c s="11" t="n" r="F17">
+      <c t="n" s="19" r="F17">
         <v>11.65</v>
       </c>
-      <c s="12" t="n" r="G17">
+      <c t="n" s="18" r="G17">
         <v>10.78</v>
       </c>
-      <c s="13" t="n" r="H17">
+      <c t="n" s="20" r="H17">
         <v>9.880000000000001</v>
       </c>
-      <c s="11" t="n" r="I17">
+      <c t="n" s="14" r="I17">
         <v>11.36</v>
       </c>
-      <c s="11" t="n" r="J17">
+      <c t="n" s="18" r="J17">
         <v>11.07</v>
       </c>
-      <c s="11" t="n" r="K17">
+      <c t="n" s="19" r="K17">
         <v>11.92</v>
       </c>
-      <c s="12" t="n" r="L17">
+      <c t="n" s="16" r="L17">
         <v>10.5</v>
       </c>
-      <c s="12" t="n" r="M17">
+      <c t="n" s="17" r="M17">
         <v>10.15</v>
       </c>
     </row>
@@ -1260,40 +1395,40 @@
       <c t="n" r="A18">
         <v>2006</v>
       </c>
-      <c s="12" t="n" r="B18">
+      <c t="n" s="18" r="B18">
         <v>10.81</v>
       </c>
-      <c s="11" t="n" r="C18">
+      <c t="n" s="18" r="C18">
         <v>11.13</v>
       </c>
-      <c s="12" t="n" r="D18">
+      <c t="n" s="16" r="D18">
         <v>10.53</v>
       </c>
-      <c s="11" t="n" r="E18">
+      <c t="n" s="18" r="E18">
         <v>11.02</v>
       </c>
-      <c s="11" t="n" r="F18">
+      <c t="n" s="14" r="F18">
         <v>11.18</v>
       </c>
-      <c s="10" t="n" r="G18">
+      <c t="n" s="13" r="G18">
         <v>12.74</v>
       </c>
-      <c s="10" t="n" r="H18">
+      <c t="n" s="13" r="H18">
         <v>12.74</v>
       </c>
-      <c s="11" t="n" r="I18">
+      <c t="n" s="19" r="I18">
         <v>11.57</v>
       </c>
-      <c s="12" t="n" r="J18">
+      <c t="n" s="16" r="J18">
         <v>10.74</v>
       </c>
-      <c s="12" t="n" r="K18">
+      <c t="n" s="16" r="K18">
         <v>10.44</v>
       </c>
-      <c s="13" t="n" r="L18">
+      <c t="n" s="20" r="L18">
         <v>9.81</v>
       </c>
-      <c s="13" t="n" r="M18">
+      <c t="n" s="20" r="M18">
         <v>9.390000000000001</v>
       </c>
     </row>
@@ -1301,40 +1436,40 @@
       <c t="n" r="A19">
         <v>2007</v>
       </c>
-      <c s="13" t="n" r="B19">
+      <c t="n" s="20" r="B19">
         <v>9.869999999999999</v>
       </c>
-      <c s="13" t="n" r="C19">
+      <c t="n" s="20" r="C19">
         <v>9.699999999999999</v>
       </c>
-      <c s="11" t="n" r="D19">
+      <c t="n" s="14" r="D19">
         <v>11.21</v>
       </c>
-      <c s="11" t="n" r="E19">
+      <c t="n" s="14" r="E19">
         <v>11.46</v>
       </c>
-      <c s="10" t="n" r="F19">
+      <c t="n" s="21" r="F19">
         <v>12.08</v>
       </c>
-      <c s="10" t="n" r="G19">
+      <c t="n" s="15" r="G19">
         <v>12.43</v>
       </c>
-      <c s="9" t="n" r="H19">
+      <c t="n" s="9" r="H19">
         <v>14.62</v>
       </c>
-      <c s="3" t="n" r="I19">
+      <c t="n" s="3" r="I19">
         <v>19.33</v>
       </c>
-      <c s="4" t="n" r="J19">
+      <c t="n" s="31" r="J19">
         <v>16.91</v>
       </c>
-      <c s="4" t="n" r="K19">
+      <c t="n" s="28" r="K19">
         <v>16.08</v>
       </c>
-      <c s="4" t="n" r="L19">
+      <c t="n" s="4" r="L19">
         <v>17.38</v>
       </c>
-      <c s="14" t="n" r="M19">
+      <c t="n" s="25" r="M19">
         <v>18.28</v>
       </c>
     </row>
@@ -1342,40 +1477,40 @@
       <c t="n" r="A20">
         <v>2008</v>
       </c>
-      <c s="2" t="n" r="B20">
+      <c t="n" s="2" r="B20">
         <v>21.79</v>
       </c>
-      <c s="2" t="n" r="C20">
+      <c t="n" s="2" r="C20">
         <v>21.64</v>
       </c>
-      <c s="16" t="n" r="D20">
+      <c t="n" s="32" r="D20">
         <v>23.3</v>
       </c>
-      <c s="3" t="n" r="E20">
+      <c t="n" s="3" r="E20">
         <v>19.21</v>
       </c>
-      <c s="4" t="n" r="F20">
+      <c t="n" s="5" r="F20">
         <v>15.82</v>
       </c>
-      <c s="4" t="n" r="G20">
+      <c t="n" s="4" r="G20">
         <v>17.56</v>
       </c>
-      <c s="3" t="n" r="H20">
+      <c t="n" s="3" r="H20">
         <v>19.65</v>
       </c>
-      <c s="14" t="n" r="I20">
+      <c t="n" s="25" r="I20">
         <v>18.64</v>
       </c>
-      <c s="3" t="n" r="J20">
+      <c t="n" s="3" r="J20">
         <v>19.43</v>
       </c>
-      <c s="5" t="n" r="K20">
+      <c t="n" s="7" r="K20">
         <v>39.39</v>
       </c>
-      <c s="5" t="n" r="L20">
+      <c t="n" s="7" r="L20">
         <v>44.25</v>
       </c>
-      <c s="5" t="n" r="M20">
+      <c t="n" s="7" r="M20">
         <v>37.96</v>
       </c>
     </row>
@@ -1383,40 +1518,40 @@
       <c t="n" r="A21">
         <v>2009</v>
       </c>
-      <c s="5" t="n" r="B21">
+      <c t="n" s="7" r="B21">
         <v>33.76</v>
       </c>
-      <c s="5" t="n" r="C21">
+      <c t="n" s="7" r="C21">
         <v>40.73</v>
       </c>
-      <c s="5" t="n" r="D21">
+      <c t="n" s="7" r="D21">
         <v>38.79</v>
       </c>
-      <c s="5" t="n" r="E21">
+      <c t="n" s="7" r="E21">
         <v>33.68</v>
       </c>
-      <c s="7" t="n" r="F21">
+      <c t="n" s="8" r="F21">
         <v>26.57</v>
       </c>
-      <c s="1" t="n" r="G21">
+      <c t="n" s="29" r="G21">
         <v>25.02</v>
       </c>
-      <c s="6" t="n" r="H21">
+      <c t="n" s="32" r="H21">
         <v>23</v>
       </c>
-      <c s="6" t="n" r="I21">
+      <c t="n" s="32" r="I21">
         <v>22.58</v>
       </c>
-      <c s="6" t="n" r="J21">
+      <c t="n" s="2" r="J21">
         <v>22.19</v>
       </c>
-      <c s="8" t="n" r="K21">
+      <c t="n" s="27" r="K21">
         <v>20.1</v>
       </c>
-      <c s="8" t="n" r="L21">
+      <c t="n" s="27" r="L21">
         <v>20.05</v>
       </c>
-      <c s="3" t="n" r="M21">
+      <c t="n" s="3" r="M21">
         <v>19.25</v>
       </c>
     </row>
@@ -1424,40 +1559,40 @@
       <c t="n" r="A22">
         <v>2010</v>
       </c>
-      <c s="4" t="n" r="B22">
+      <c t="n" s="31" r="B22">
         <v>16.86</v>
       </c>
-      <c s="3" t="n" r="C22">
+      <c t="n" s="3" r="C22">
         <v>19.32</v>
       </c>
-      <c s="4" t="n" r="D22">
+      <c t="n" s="28" r="D22">
         <v>16.17</v>
       </c>
-      <c s="4" t="n" r="E22">
+      <c t="n" s="10" r="E22">
         <v>15.23</v>
       </c>
-      <c s="14" t="n" r="F22">
+      <c t="n" s="25" r="F22">
         <v>18.41</v>
       </c>
-      <c s="6" t="n" r="G22">
+      <c t="n" s="32" r="G22">
         <v>22.87</v>
       </c>
-      <c s="2" t="n" r="H22">
+      <c t="n" s="2" r="H22">
         <v>21.86</v>
       </c>
-      <c s="2" t="n" r="I22">
+      <c t="n" s="6" r="I22">
         <v>21.36</v>
       </c>
-      <c s="8" t="n" r="J22">
+      <c t="n" s="6" r="J22">
         <v>20.85</v>
       </c>
-      <c s="4" t="n" r="K22">
+      <c t="n" s="26" r="K22">
         <v>17.9</v>
       </c>
-      <c s="4" t="n" r="L22">
+      <c t="n" s="26" r="L22">
         <v>17.76</v>
       </c>
-      <c s="4" t="n" r="M22">
+      <c t="n" s="10" r="M22">
         <v>15.4</v>
       </c>
     </row>
@@ -1465,40 +1600,40 @@
       <c t="n" r="A23">
         <v>2011</v>
       </c>
-      <c s="4" t="n" r="B23">
+      <c t="n" s="10" r="B23">
         <v>15.37</v>
       </c>
-      <c s="9" t="n" r="C23">
+      <c t="n" s="9" r="C23">
         <v>14.86</v>
       </c>
-      <c s="4" t="n" r="D23">
+      <c t="n" s="31" r="D23">
         <v>17.07</v>
       </c>
-      <c s="9" t="n" r="E23">
+      <c t="n" s="11" r="E23">
         <v>14.27</v>
       </c>
-      <c s="9" t="n" r="F23">
+      <c t="n" s="11" r="F23">
         <v>14.49</v>
       </c>
-      <c s="4" t="n" r="G23">
+      <c t="n" s="28" r="G23">
         <v>15.88</v>
       </c>
-      <c s="4" t="n" r="H23">
+      <c t="n" s="10" r="H23">
         <v>15.12</v>
       </c>
-      <c s="6" t="n" r="I23">
+      <c t="n" s="2" r="I23">
         <v>22.46</v>
       </c>
-      <c s="5" t="n" r="J23">
+      <c t="n" s="7" r="J23">
         <v>30.43</v>
       </c>
-      <c s="17" t="n" r="K23">
+      <c t="n" s="29" r="K23">
         <v>24.44</v>
       </c>
-      <c s="15" t="n" r="L23">
+      <c t="n" s="8" r="L23">
         <v>27.03</v>
       </c>
-      <c s="8" t="n" r="M23">
+      <c t="n" s="27" r="M23">
         <v>20.34</v>
       </c>
     </row>
@@ -1506,40 +1641,40 @@
       <c t="n" r="A24">
         <v>2012</v>
       </c>
-      <c s="4" t="n" r="B24">
+      <c t="n" s="31" r="B24">
         <v>16.8</v>
       </c>
-      <c s="4" t="n" r="C24">
+      <c t="n" s="28" r="C24">
         <v>16.1</v>
       </c>
-      <c s="9" t="n" r="D24">
+      <c t="n" s="22" r="D24">
         <v>13.66</v>
       </c>
-      <c s="9" t="n" r="E24">
+      <c t="n" s="9" r="E24">
         <v>14.67</v>
       </c>
-      <c s="4" t="n" r="F24">
+      <c t="n" s="28" r="F24">
         <v>16.01</v>
       </c>
-      <c s="4" t="n" r="G24">
+      <c t="n" s="31" r="G24">
         <v>16.77</v>
       </c>
-      <c s="4" t="n" r="H24">
+      <c t="n" s="5" r="H24">
         <v>15.45</v>
       </c>
-      <c s="9" t="n" r="I24">
+      <c t="n" s="23" r="I24">
         <v>13.3</v>
       </c>
-      <c s="9" t="n" r="J24">
+      <c t="n" s="22" r="J24">
         <v>13.51</v>
       </c>
-      <c s="9" t="n" r="K24">
+      <c t="n" s="22" r="K24">
         <v>13.67</v>
       </c>
-      <c s="9" t="n" r="L24">
+      <c t="n" s="9" r="L24">
         <v>14.77</v>
       </c>
-      <c s="9" t="n" r="M24">
+      <c t="n" s="9" r="M24">
         <v>14.89</v>
       </c>
     </row>
@@ -1547,40 +1682,40 @@
       <c t="n" r="A25">
         <v>2013</v>
       </c>
-      <c s="10" t="n" r="B25">
+      <c t="n" s="21" r="B25">
         <v>12.29</v>
       </c>
-      <c s="10" t="n" r="C25">
+      <c t="n" s="21" r="C25">
         <v>12.08</v>
       </c>
-      <c s="11" t="n" r="D25">
+      <c t="n" s="18" r="D25">
         <v>11.05</v>
       </c>
-      <c s="11" t="n" r="E25">
+      <c t="n" s="21" r="E25">
         <v>11.99</v>
       </c>
-      <c s="10" t="n" r="F25">
+      <c t="n" s="21" r="F25">
         <v>12.26</v>
       </c>
-      <c s="9" t="n" r="G25">
+      <c t="n" s="11" r="G25">
         <v>14.36</v>
       </c>
-      <c s="10" t="n" r="H25">
+      <c t="n" s="21" r="H25">
         <v>12.07</v>
       </c>
-      <c s="11" t="n" r="I25">
+      <c t="n" s="19" r="I25">
         <v>11.83</v>
       </c>
-      <c s="10" t="n" r="J25">
+      <c t="n" s="15" r="J25">
         <v>12.52</v>
       </c>
-      <c s="10" t="n" r="K25">
+      <c t="n" s="15" r="K25">
         <v>12.34</v>
       </c>
-      <c s="11" t="n" r="L25">
+      <c t="n" s="21" r="L25">
         <v>11.99</v>
       </c>
-      <c s="11" t="n" r="M25">
+      <c t="n" s="19" r="M25">
         <v>11.69</v>
       </c>
     </row>
@@ -1588,44 +1723,44 @@
       <c t="n" r="A26">
         <v>2014</v>
       </c>
-      <c s="11" t="n" r="B26">
+      <c t="n" s="19" r="B26">
         <v>11.81</v>
       </c>
-      <c s="9" t="n" r="C26">
+      <c t="n" s="23" r="C26">
         <v>13.44</v>
       </c>
-      <c s="9" t="n" r="D26">
+      <c t="n" s="23" r="D26">
         <v>13.46</v>
       </c>
-      <c s="10" t="n" r="E26">
+      <c t="n" s="15" r="E26">
         <v>12.6</v>
       </c>
-      <c s="11" t="n" r="F26">
+      <c t="n" s="14" r="F26">
         <v>11.32</v>
       </c>
-      <c s="12" t="n" r="G26">
+      <c t="n" s="17" r="G26">
         <v>10.34</v>
       </c>
-      <c s="12" t="n" r="H26">
+      <c t="n" s="17" r="H26">
         <v>10.28</v>
       </c>
-      <c s="11" t="n" r="I26">
+      <c t="n" s="14" r="I26">
         <v>11.24</v>
       </c>
-      <c s="11" t="n" r="J26">
+      <c t="n" s="14" r="J26">
         <v>11.52</v>
       </c>
-      <c s="9" t="n" r="K26">
+      <c t="n" s="22" r="K26">
         <v>13.72</v>
       </c>
-      <c s="11" t="n" r="L26">
+      <c t="n" s="19" r="L26">
         <v>11.91</v>
       </c>
-      <c s="11" t="n" r="M26">
+      <c t="n" s="14" r="M26">
         <v>11.53</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" left="0.75" right="0.75" bottom="1" footer="0.5" header="0.5"/>
+  <pageMargins top="1" footer="0.5" header="0.5" bottom="1" left="0.75" right="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed more color spectrum bugs
</commit_message>
<xml_diff>
--- a/All_Lows.xlsx
+++ b/All_Lows.xlsx
@@ -76,194 +76,194 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00FF1000"/>
+        <bgColor rgb="00FF1000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF3000"/>
+        <bgColor rgb="00FF3000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF4800"/>
+        <bgColor rgb="00FF4800"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFE700"/>
+        <bgColor rgb="00FFE700"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EFFF00"/>
+        <bgColor rgb="00EFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF3800"/>
+        <bgColor rgb="00FF3800"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0800"/>
+        <bgColor rgb="00FF0800"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DFFF00"/>
+        <bgColor rgb="00DFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E7FF00"/>
+        <bgColor rgb="00E7FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0060FF00"/>
+        <bgColor rgb="0060FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0058FF00"/>
+        <bgColor rgb="0058FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0040FF00"/>
+        <bgColor rgb="0040FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0020FF00"/>
+        <bgColor rgb="0020FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0038FF00"/>
+        <bgColor rgb="0038FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0010FF00"/>
+        <bgColor rgb="0010FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0008FF00"/>
+        <bgColor rgb="0008FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0018FF00"/>
+        <bgColor rgb="0018FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0028FF00"/>
+        <bgColor rgb="0028FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000FF00"/>
+        <bgColor rgb="0000FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0030FF00"/>
+        <bgColor rgb="0030FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0050FF00"/>
+        <bgColor rgb="0050FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0048FF00"/>
+        <bgColor rgb="0048FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF700"/>
+        <bgColor rgb="00FFF700"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF5000"/>
+        <bgColor rgb="00FF5000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFDF00"/>
+        <bgColor rgb="00FFDF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF4000"/>
+        <bgColor rgb="00FF4000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F7FF00"/>
+        <bgColor rgb="00F7FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF1800"/>
+        <bgColor rgb="00FF1800"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00FF2000"/>
         <bgColor rgb="00FF2000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF4000"/>
-        <bgColor rgb="00FF4000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF5800"/>
-        <bgColor rgb="00FF5800"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00FFEF00"/>
         <bgColor rgb="00FFEF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00E7FF00"/>
-        <bgColor rgb="00E7FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF4800"/>
-        <bgColor rgb="00FF4800"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF1000"/>
-        <bgColor rgb="00FF1000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF1800"/>
-        <bgColor rgb="00FF1800"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0068FF00"/>
-        <bgColor rgb="0068FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00DFFF00"/>
-        <bgColor rgb="00DFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0060FF00"/>
-        <bgColor rgb="0060FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0058FF00"/>
-        <bgColor rgb="0058FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0040FF00"/>
-        <bgColor rgb="0040FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0020FF00"/>
-        <bgColor rgb="0020FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0038FF00"/>
-        <bgColor rgb="0038FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0010FF00"/>
-        <bgColor rgb="0010FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0008FF00"/>
-        <bgColor rgb="0008FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0018FF00"/>
-        <bgColor rgb="0018FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0028FF00"/>
-        <bgColor rgb="0028FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0000FF00"/>
-        <bgColor rgb="0000FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0030FF00"/>
-        <bgColor rgb="0030FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0050FF00"/>
-        <bgColor rgb="0050FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0048FF00"/>
-        <bgColor rgb="0048FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F7FF00"/>
-        <bgColor rgb="00F7FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFDF00"/>
-        <bgColor rgb="00FFDF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFE700"/>
-        <bgColor rgb="00FFE700"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF5000"/>
-        <bgColor rgb="00FF5000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00EFFF00"/>
-        <bgColor rgb="00EFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00FF2800"/>
         <bgColor rgb="00FF2800"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF3000"/>
-        <bgColor rgb="00FF3000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFF700"/>
-        <bgColor rgb="00FFF700"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF3800"/>
-        <bgColor rgb="00FF3800"/>
       </patternFill>
     </fill>
   </fills>
@@ -685,7 +685,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -697,7 +697,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row spans="1:13" r="1">
+    <row r="1" spans="1:13">
       <c t="s" r="B1">
         <v>0</v>
       </c>
@@ -735,1032 +735,1032 @@
         <v>11</v>
       </c>
     </row>
-    <row spans="1:13" r="2">
+    <row r="2" spans="1:13">
       <c t="n" r="A2">
         <v>1990</v>
       </c>
-      <c t="n" s="1" r="B2">
+      <c t="n" r="B2" s="1">
         <v>25.36</v>
       </c>
-      <c t="n" s="2" r="C2">
+      <c t="n" r="C2" s="2">
         <v>21.99</v>
       </c>
-      <c t="n" s="3" r="D2">
+      <c t="n" r="D2" s="3">
         <v>19.73</v>
       </c>
-      <c t="n" s="3" r="E2">
+      <c t="n" r="E2" s="3">
         <v>19.52</v>
       </c>
-      <c t="n" s="4" r="F2">
+      <c t="n" r="F2" s="4">
         <v>17.37</v>
       </c>
-      <c t="n" s="5" r="G2">
+      <c t="n" r="G2" s="5">
         <v>15.5</v>
       </c>
-      <c t="n" s="6" r="H2">
+      <c t="n" r="H2" s="6">
         <v>21.11</v>
       </c>
-      <c t="n" s="7" r="I2">
+      <c t="n" r="I2" s="7">
         <v>29.9</v>
       </c>
-      <c t="n" s="7" r="J2">
+      <c t="n" r="J2" s="7">
         <v>29.11</v>
       </c>
-      <c t="n" s="7" r="K2">
+      <c t="n" r="K2" s="7">
         <v>30.04</v>
       </c>
-      <c t="n" s="2" r="L2">
+      <c t="n" r="L2" s="2">
         <v>22.16</v>
       </c>
-      <c t="n" s="8" r="M2">
+      <c t="n" r="M2" s="8">
         <v>26.38</v>
       </c>
     </row>
-    <row spans="1:13" r="3">
+    <row r="3" spans="1:13">
       <c t="n" r="A3">
         <v>1991</v>
       </c>
-      <c t="n" s="6" r="B3">
+      <c t="n" r="B3" s="6">
         <v>20.91</v>
       </c>
-      <c t="n" s="3" r="C3">
+      <c t="n" r="C3" s="3">
         <v>19.57</v>
       </c>
-      <c t="n" s="9" r="D3">
+      <c t="n" r="D3" s="9">
         <v>14.9</v>
       </c>
-      <c t="n" s="5" r="E3">
+      <c t="n" r="E3" s="5">
         <v>15.47</v>
       </c>
-      <c t="n" s="10" r="F3">
+      <c t="n" r="F3" s="10">
         <v>15.23</v>
       </c>
-      <c t="n" s="5" r="G3">
+      <c t="n" r="G3" s="5">
         <v>15.5</v>
       </c>
-      <c t="n" s="10" r="H3">
+      <c t="n" r="H3" s="10">
         <v>15.18</v>
       </c>
-      <c t="n" s="11" r="I3">
+      <c t="n" r="I3" s="11">
         <v>14.41</v>
       </c>
-      <c t="n" s="11" r="J3">
+      <c t="n" r="J3" s="11">
         <v>14.46</v>
       </c>
-      <c t="n" s="9" r="K3">
+      <c t="n" r="K3" s="9">
         <v>14.81</v>
       </c>
-      <c t="n" s="12" r="L3">
+      <c t="n" r="L3" s="12">
         <v>13.95</v>
       </c>
-      <c t="n" s="5" r="M3">
+      <c t="n" r="M3" s="5">
         <v>15.44</v>
       </c>
     </row>
-    <row spans="1:13" r="4">
+    <row r="4" spans="1:13">
       <c t="n" r="A4">
         <v>1992</v>
       </c>
-      <c t="n" s="12" r="B4">
+      <c t="n" r="B4" s="12">
         <v>14.12</v>
       </c>
-      <c t="n" s="12" r="C4">
+      <c t="n" r="C4" s="12">
         <v>14.12</v>
       </c>
-      <c t="n" s="10" r="D4">
+      <c t="n" r="D4" s="10">
         <v>15.34</v>
       </c>
-      <c t="n" s="9" r="E4">
+      <c t="n" r="E4" s="9">
         <v>14.83</v>
       </c>
-      <c t="n" s="13" r="F4">
+      <c t="n" r="F4" s="13">
         <v>12.77</v>
       </c>
-      <c t="n" s="13" r="G4">
+      <c t="n" r="G4" s="13">
         <v>12.73</v>
       </c>
-      <c t="n" s="14" r="H4">
+      <c t="n" r="H4" s="14">
         <v>11.36</v>
       </c>
-      <c t="n" s="15" r="I4">
+      <c t="n" r="I4" s="15">
         <v>12.34</v>
       </c>
-      <c t="n" s="16" r="J4">
+      <c t="n" r="J4" s="16">
         <v>10.69</v>
       </c>
-      <c t="n" s="10" r="K4">
+      <c t="n" r="K4" s="10">
         <v>15.03</v>
       </c>
-      <c t="n" s="14" r="L4">
+      <c t="n" r="L4" s="14">
         <v>11.38</v>
       </c>
-      <c t="n" s="17" r="M4">
+      <c t="n" r="M4" s="17">
         <v>10.29</v>
       </c>
     </row>
-    <row spans="1:13" r="5">
+    <row r="5" spans="1:13">
       <c t="n" r="A5">
         <v>1993</v>
       </c>
-      <c t="n" s="18" r="B5">
+      <c t="n" r="B5" s="18">
         <v>10.98</v>
       </c>
-      <c t="n" s="19" r="C5">
+      <c t="n" r="C5" s="19">
         <v>11.69</v>
       </c>
-      <c t="n" s="16" r="D5">
+      <c t="n" r="D5" s="16">
         <v>10.66</v>
       </c>
-      <c t="n" s="16" r="E5">
+      <c t="n" r="E5" s="16">
         <v>10.71</v>
       </c>
-      <c t="n" s="14" r="F5">
+      <c t="n" r="F5" s="14">
         <v>11.25</v>
       </c>
-      <c t="n" s="18" r="G5">
+      <c t="n" r="G5" s="18">
         <v>10.86</v>
       </c>
-      <c t="n" s="20" r="H5">
+      <c t="n" r="H5" s="20">
         <v>9.109999999999999</v>
       </c>
-      <c t="n" s="17" r="I5">
+      <c t="n" r="I5" s="17">
         <v>10.34</v>
       </c>
-      <c t="n" s="16" r="J5">
+      <c t="n" r="J5" s="16">
         <v>10.75</v>
       </c>
-      <c t="n" s="17" r="K5">
+      <c t="n" r="K5" s="17">
         <v>10</v>
       </c>
-      <c t="n" s="14" r="L5">
+      <c t="n" r="L5" s="14">
         <v>11.49</v>
       </c>
-      <c t="n" s="20" r="M5">
+      <c t="n" r="M5" s="20">
         <v>8.890000000000001</v>
       </c>
     </row>
-    <row spans="1:13" r="6">
+    <row r="6" spans="1:13">
       <c t="n" r="A6">
         <v>1994</v>
       </c>
-      <c t="n" s="20" r="B6">
+      <c t="n" r="B6" s="20">
         <v>9.59</v>
       </c>
-      <c t="n" s="17" r="C6">
+      <c t="n" r="C6" s="17">
         <v>10.21</v>
       </c>
-      <c t="n" s="19" r="D6">
+      <c t="n" r="D6" s="19">
         <v>11.58</v>
       </c>
-      <c t="n" s="13" r="E6">
+      <c t="n" r="E6" s="13">
         <v>13.05</v>
       </c>
-      <c t="n" s="14" r="F6">
+      <c t="n" r="F6" s="14">
         <v>11.44</v>
       </c>
-      <c t="n" s="16" r="G6">
+      <c t="n" r="G6" s="16">
         <v>10.48</v>
       </c>
-      <c t="n" s="18" r="H6">
+      <c t="n" r="H6" s="18">
         <v>10.96</v>
       </c>
-      <c t="n" s="16" r="I6">
+      <c t="n" r="I6" s="16">
         <v>10.75</v>
       </c>
-      <c t="n" s="14" r="J6">
+      <c t="n" r="J6" s="14">
         <v>11.17</v>
       </c>
-      <c t="n" s="13" r="K6">
+      <c t="n" r="K6" s="13">
         <v>12.75</v>
       </c>
-      <c t="n" s="11" r="L6">
+      <c t="n" r="L6" s="11">
         <v>14.32</v>
       </c>
-      <c t="n" s="14" r="M6">
+      <c t="n" r="M6" s="14">
         <v>11.36</v>
       </c>
     </row>
-    <row spans="1:13" r="7">
+    <row r="7" spans="1:13">
       <c t="n" r="A7">
         <v>1995</v>
       </c>
-      <c t="n" s="16" r="B7">
+      <c t="n" r="B7" s="16">
         <v>10.76</v>
       </c>
-      <c t="n" s="16" r="C7">
+      <c t="n" r="C7" s="16">
         <v>10.51</v>
       </c>
-      <c t="n" s="18" r="D7">
+      <c t="n" r="D7" s="18">
         <v>10.79</v>
       </c>
-      <c t="n" s="18" r="E7">
+      <c t="n" r="E7" s="18">
         <v>10.95</v>
       </c>
-      <c t="n" s="17" r="F7">
+      <c t="n" r="F7" s="17">
         <v>10.08</v>
       </c>
-      <c t="n" s="17" r="G7">
+      <c t="n" r="G7" s="17">
         <v>10.36</v>
       </c>
-      <c t="n" s="16" r="H7">
+      <c t="n" r="H7" s="16">
         <v>10.75</v>
       </c>
-      <c t="n" s="14" r="I7">
+      <c t="n" r="I7" s="14">
         <v>11.36</v>
       </c>
-      <c t="n" s="17" r="J7">
+      <c t="n" r="J7" s="17">
         <v>10.19</v>
       </c>
-      <c t="n" s="21" r="K7">
+      <c t="n" r="K7" s="21">
         <v>12.09</v>
       </c>
-      <c t="n" s="16" r="L7">
+      <c t="n" r="L7" s="16">
         <v>10.57</v>
       </c>
-      <c t="n" s="17" r="M7">
+      <c t="n" r="M7" s="17">
         <v>10.06</v>
       </c>
     </row>
-    <row spans="1:13" r="8">
+    <row r="8" spans="1:13">
       <c t="n" r="A8">
         <v>1996</v>
       </c>
-      <c t="n" s="14" r="B8">
+      <c t="n" r="B8" s="14">
         <v>11.23</v>
       </c>
-      <c t="n" s="18" r="C8">
+      <c t="n" r="C8" s="18">
         <v>11.11</v>
       </c>
-      <c t="n" s="9" r="D8">
+      <c t="n" r="D8" s="9">
         <v>14.98</v>
       </c>
-      <c t="n" s="12" r="E8">
+      <c t="n" r="E8" s="12">
         <v>13.99</v>
       </c>
-      <c t="n" s="11" r="F8">
+      <c t="n" r="F8" s="11">
         <v>14.56</v>
       </c>
-      <c t="n" s="22" r="G8">
+      <c t="n" r="G8" s="22">
         <v>13.55</v>
       </c>
-      <c t="n" s="22" r="H8">
+      <c t="n" r="H8" s="22">
         <v>13.75</v>
       </c>
-      <c t="n" s="23" r="I8">
+      <c t="n" r="I8" s="23">
         <v>13.22</v>
       </c>
-      <c t="n" s="11" r="J8">
+      <c t="n" r="J8" s="11">
         <v>14.55</v>
       </c>
-      <c t="n" s="9" r="K8">
+      <c t="n" r="K8" s="9">
         <v>14.63</v>
       </c>
-      <c t="n" s="23" r="L8">
+      <c t="n" r="L8" s="23">
         <v>13.45</v>
       </c>
-      <c t="n" s="24" r="M8">
+      <c t="n" r="M8" s="24">
         <v>16.68</v>
       </c>
     </row>
-    <row spans="1:13" r="9">
+    <row r="9" spans="1:13">
       <c t="n" r="A9">
         <v>1997</v>
       </c>
-      <c t="n" s="24" r="B9">
+      <c t="n" r="B9" s="24">
         <v>16.36</v>
       </c>
-      <c t="n" s="25" r="C9">
+      <c t="n" r="C9" s="25">
         <v>18.71</v>
       </c>
-      <c t="n" s="4" r="D9">
+      <c t="n" r="D9" s="4">
         <v>17.3</v>
       </c>
-      <c t="n" s="4" r="E9">
+      <c t="n" r="E9" s="4">
         <v>17.57</v>
       </c>
-      <c t="n" s="4" r="F9">
+      <c t="n" r="F9" s="4">
         <v>17.28</v>
       </c>
-      <c t="n" s="25" r="G9">
+      <c t="n" r="G9" s="25">
         <v>18.2</v>
       </c>
-      <c t="n" s="26" r="H9">
+      <c t="n" r="H9" s="26">
         <v>17.82</v>
       </c>
-      <c t="n" s="3" r="I9">
+      <c t="n" r="I9" s="3">
         <v>19.33</v>
       </c>
-      <c t="n" s="6" r="J9">
+      <c t="n" r="J9" s="6">
         <v>21.43</v>
       </c>
-      <c t="n" s="3" r="K9">
+      <c t="n" r="K9" s="3">
         <v>19.28</v>
       </c>
-      <c t="n" s="8" r="L9">
+      <c t="n" r="L9" s="8">
         <v>26.42</v>
       </c>
-      <c t="n" s="27" r="M9">
+      <c t="n" r="M9" s="27">
         <v>20.41</v>
       </c>
     </row>
-    <row spans="1:13" r="10">
+    <row r="10" spans="1:13">
       <c t="n" r="A10">
         <v>1998</v>
       </c>
-      <c t="n" s="27" r="B10">
+      <c t="n" r="B10" s="27">
         <v>20.55</v>
       </c>
-      <c t="n" s="25" r="C10">
+      <c t="n" r="C10" s="25">
         <v>18.39</v>
       </c>
-      <c t="n" s="26" r="D10">
+      <c t="n" r="D10" s="26">
         <v>17.58</v>
       </c>
-      <c t="n" s="3" r="E10">
+      <c t="n" r="E10" s="3">
         <v>19.25</v>
       </c>
-      <c t="n" s="25" r="F10">
+      <c t="n" r="F10" s="25">
         <v>18.6</v>
       </c>
-      <c t="n" s="3" r="G10">
+      <c t="n" r="G10" s="3">
         <v>18.93</v>
       </c>
-      <c t="n" s="28" r="H10">
+      <c t="n" r="H10" s="28">
         <v>16.1</v>
       </c>
-      <c t="n" s="2" r="I10">
+      <c t="n" r="I10" s="2">
         <v>22.11</v>
       </c>
-      <c t="n" s="7" r="J10">
+      <c t="n" r="J10" s="7">
         <v>32.44</v>
       </c>
-      <c t="n" s="7" r="K10">
+      <c t="n" r="K10" s="7">
         <v>27.54</v>
       </c>
-      <c t="n" s="6" r="L10">
+      <c t="n" r="L10" s="6">
         <v>21.24</v>
       </c>
-      <c t="n" s="27" r="M10">
+      <c t="n" r="M10" s="27">
         <v>20.08</v>
       </c>
     </row>
-    <row spans="1:13" r="11">
+    <row r="11" spans="1:13">
       <c t="n" r="A11">
         <v>1999</v>
       </c>
-      <c t="n" s="6" r="B11">
+      <c t="n" r="B11" s="6">
         <v>21.38</v>
       </c>
-      <c t="n" s="29" r="C11">
+      <c t="n" r="C11" s="29">
         <v>25.22</v>
       </c>
-      <c t="n" s="2" r="D11">
+      <c t="n" r="D11" s="2">
         <v>22</v>
       </c>
-      <c t="n" s="27" r="E11">
+      <c t="n" r="E11" s="27">
         <v>20.47</v>
       </c>
-      <c t="n" s="30" r="F11">
+      <c t="n" r="F11" s="30">
         <v>23.62</v>
       </c>
-      <c t="n" s="27" r="G11">
+      <c t="n" r="G11" s="27">
         <v>20.67</v>
       </c>
-      <c t="n" s="31" r="H11">
+      <c t="n" r="H11" s="31">
         <v>17.07</v>
       </c>
-      <c t="n" s="27" r="I11">
+      <c t="n" r="I11" s="27">
         <v>20.12</v>
       </c>
-      <c t="n" s="6" r="J11">
+      <c t="n" r="J11" s="6">
         <v>20.87</v>
       </c>
-      <c t="n" s="27" r="K11">
+      <c t="n" r="K11" s="27">
         <v>20.3</v>
       </c>
-      <c t="n" s="25" r="L11">
+      <c t="n" r="L11" s="25">
         <v>18.64</v>
       </c>
-      <c t="n" s="25" r="M11">
+      <c t="n" r="M11" s="25">
         <v>18.69</v>
       </c>
     </row>
-    <row spans="1:13" r="12">
+    <row r="12" spans="1:13">
       <c t="n" r="A12">
         <v>2000</v>
       </c>
-      <c t="n" s="3" r="B12">
+      <c t="n" r="B12" s="3">
         <v>19.51</v>
       </c>
-      <c t="n" s="27" r="C12">
+      <c t="n" r="C12" s="27">
         <v>20.69</v>
       </c>
-      <c t="n" s="3" r="D12">
+      <c t="n" r="D12" s="3">
         <v>19.19</v>
       </c>
-      <c t="n" s="32" r="E12">
+      <c t="n" r="E12" s="32">
         <v>23.25</v>
       </c>
-      <c t="n" s="32" r="F12">
+      <c t="n" r="F12" s="32">
         <v>23.23</v>
       </c>
-      <c t="n" s="3" r="G12">
+      <c t="n" r="G12" s="3">
         <v>19.39</v>
       </c>
-      <c t="n" s="25" r="H12">
+      <c t="n" r="H12" s="25">
         <v>18.77</v>
       </c>
-      <c t="n" s="28" r="I12">
+      <c t="n" r="I12" s="28">
         <v>16.28</v>
       </c>
-      <c t="n" s="24" r="J12">
+      <c t="n" r="J12" s="24">
         <v>16.47</v>
       </c>
-      <c t="n" s="3" r="K12">
+      <c t="n" r="K12" s="3">
         <v>19.8</v>
       </c>
-      <c t="n" s="30" r="L12">
+      <c t="n" r="L12" s="30">
         <v>23.51</v>
       </c>
-      <c t="n" s="2" r="M12">
+      <c t="n" r="M12" s="2">
         <v>22.38</v>
       </c>
     </row>
-    <row spans="1:13" r="13">
+    <row r="13" spans="1:13">
       <c t="n" r="A13">
         <v>2001</v>
       </c>
-      <c t="n" s="6" r="B13">
+      <c t="n" r="B13" s="6">
         <v>21.47</v>
       </c>
-      <c t="n" s="27" r="C13">
+      <c t="n" r="C13" s="27">
         <v>20.22</v>
       </c>
-      <c t="n" s="30" r="D13">
+      <c t="n" r="D13" s="30">
         <v>24.12</v>
       </c>
-      <c t="n" s="32" r="E13">
+      <c t="n" r="E13" s="32">
         <v>23.01</v>
       </c>
-      <c t="n" s="27" r="F13">
+      <c t="n" r="F13" s="27">
         <v>20.46</v>
       </c>
-      <c t="n" s="25" r="G13">
+      <c t="n" r="G13" s="25">
         <v>18.83</v>
       </c>
-      <c t="n" s="25" r="H13">
+      <c t="n" r="H13" s="25">
         <v>18.74</v>
       </c>
-      <c t="n" s="3" r="I13">
+      <c t="n" r="I13" s="3">
         <v>19.69</v>
       </c>
-      <c t="n" s="30" r="J13">
+      <c t="n" r="J13" s="30">
         <v>24.19</v>
       </c>
-      <c t="n" s="7" r="K13">
+      <c t="n" r="K13" s="7">
         <v>28.11</v>
       </c>
-      <c t="n" s="32" r="L13">
+      <c t="n" r="L13" s="32">
         <v>22.96</v>
       </c>
-      <c t="n" s="6" r="M13">
+      <c t="n" r="M13" s="6">
         <v>21.12</v>
       </c>
     </row>
-    <row spans="1:13" r="14">
+    <row r="14" spans="1:13">
       <c t="n" r="A14">
         <v>2002</v>
       </c>
-      <c t="n" s="27" r="B14">
+      <c t="n" r="B14" s="27">
         <v>20.4</v>
       </c>
-      <c t="n" s="27" r="C14">
+      <c t="n" r="C14" s="27">
         <v>20.55</v>
       </c>
-      <c t="n" s="31" r="D14">
+      <c t="n" r="D14" s="31">
         <v>17.02</v>
       </c>
-      <c t="n" s="26" r="E14">
+      <c t="n" r="E14" s="26">
         <v>17.73</v>
       </c>
-      <c t="n" s="26" r="F14">
+      <c t="n" r="F14" s="26">
         <v>17.7</v>
       </c>
-      <c t="n" s="3" r="G14">
+      <c t="n" r="G14" s="3">
         <v>19.43</v>
       </c>
-      <c t="n" s="1" r="H14">
+      <c t="n" r="H14" s="1">
         <v>25.63</v>
       </c>
-      <c t="n" s="7" r="I14">
+      <c t="n" r="I14" s="7">
         <v>27.61</v>
       </c>
-      <c t="n" s="7" r="J14">
+      <c t="n" r="J14" s="7">
         <v>31.93</v>
       </c>
-      <c t="n" s="7" r="K14">
+      <c t="n" r="K14" s="7">
         <v>29.69</v>
       </c>
-      <c t="n" s="32" r="L14">
+      <c t="n" r="L14" s="32">
         <v>23.05</v>
       </c>
-      <c t="n" s="1" r="M14">
+      <c t="n" r="M14" s="1">
         <v>25.87</v>
       </c>
     </row>
-    <row spans="1:13" r="15">
+    <row r="15" spans="1:13">
       <c t="n" r="A15">
         <v>2003</v>
       </c>
-      <c t="n" s="30" r="B15">
+      <c t="n" r="B15" s="30">
         <v>24.02</v>
       </c>
-      <c t="n" s="7" r="C15">
+      <c t="n" r="C15" s="7">
         <v>29.06</v>
       </c>
-      <c t="n" s="7" r="D15">
+      <c t="n" r="D15" s="7">
         <v>27.58</v>
       </c>
-      <c t="n" s="27" r="E15">
+      <c t="n" r="E15" s="27">
         <v>20.26</v>
       </c>
-      <c t="n" s="25" r="F15">
+      <c t="n" r="F15" s="25">
         <v>18.24</v>
       </c>
-      <c t="n" s="25" r="G15">
+      <c t="n" r="G15" s="25">
         <v>18.87</v>
       </c>
-      <c t="n" s="26" r="H15">
+      <c t="n" r="H15" s="26">
         <v>17.65</v>
       </c>
-      <c t="n" s="26" r="I15">
+      <c t="n" r="I15" s="26">
         <v>17.64</v>
       </c>
-      <c t="n" s="4" r="J15">
+      <c t="n" r="J15" s="4">
         <v>17.52</v>
       </c>
-      <c t="n" s="5" r="K15">
+      <c t="n" r="K15" s="5">
         <v>15.79</v>
       </c>
-      <c t="n" s="5" r="L15">
+      <c t="n" r="L15" s="5">
         <v>15.79</v>
       </c>
-      <c t="n" s="9" r="M15">
+      <c t="n" r="M15" s="9">
         <v>14.66</v>
       </c>
     </row>
-    <row spans="1:13" r="16">
+    <row r="16" spans="1:13">
       <c t="n" r="A16">
         <v>2004</v>
       </c>
-      <c t="n" s="12" r="B16">
+      <c t="n" r="B16" s="12">
         <v>14.01</v>
       </c>
-      <c t="n" s="22" r="C16">
+      <c t="n" r="C16" s="22">
         <v>13.8</v>
       </c>
-      <c t="n" s="22" r="D16">
+      <c t="n" r="D16" s="22">
         <v>13.83</v>
       </c>
-      <c t="n" s="12" r="E16">
+      <c t="n" r="E16" s="12">
         <v>13.86</v>
       </c>
-      <c t="n" s="10" r="F16">
+      <c t="n" r="F16" s="10">
         <v>15.19</v>
       </c>
-      <c t="n" s="22" r="G16">
+      <c t="n" r="G16" s="22">
         <v>13.75</v>
       </c>
-      <c t="n" s="23" r="H16">
+      <c t="n" r="H16" s="23">
         <v>13.34</v>
       </c>
-      <c t="n" s="9" r="I16">
+      <c t="n" r="I16" s="9">
         <v>14.67</v>
       </c>
-      <c t="n" s="23" r="J16">
+      <c t="n" r="J16" s="23">
         <v>13.16</v>
       </c>
-      <c t="n" s="15" r="K16">
+      <c t="n" r="K16" s="15">
         <v>12.6</v>
       </c>
-      <c t="n" s="15" r="L16">
+      <c t="n" r="L16" s="15">
         <v>12.56</v>
       </c>
-      <c t="n" s="18" r="M16">
+      <c t="n" r="M16" s="18">
         <v>11.14</v>
       </c>
     </row>
-    <row spans="1:13" r="17">
+    <row r="17" spans="1:13">
       <c t="n" r="A17">
         <v>2005</v>
       </c>
-      <c t="n" s="21" r="B17">
+      <c t="n" r="B17" s="21">
         <v>12.29</v>
       </c>
-      <c t="n" s="18" r="C17">
+      <c t="n" r="C17" s="18">
         <v>10.9</v>
       </c>
-      <c t="n" s="19" r="D17">
+      <c t="n" r="D17" s="19">
         <v>11.66</v>
       </c>
-      <c t="n" s="14" r="E17">
+      <c t="n" r="E17" s="14">
         <v>11.2</v>
       </c>
-      <c t="n" s="19" r="F17">
+      <c t="n" r="F17" s="19">
         <v>11.65</v>
       </c>
-      <c t="n" s="18" r="G17">
+      <c t="n" r="G17" s="18">
         <v>10.78</v>
       </c>
-      <c t="n" s="20" r="H17">
+      <c t="n" r="H17" s="20">
         <v>9.880000000000001</v>
       </c>
-      <c t="n" s="14" r="I17">
+      <c t="n" r="I17" s="14">
         <v>11.36</v>
       </c>
-      <c t="n" s="18" r="J17">
+      <c t="n" r="J17" s="18">
         <v>11.07</v>
       </c>
-      <c t="n" s="19" r="K17">
+      <c t="n" r="K17" s="19">
         <v>11.92</v>
       </c>
-      <c t="n" s="16" r="L17">
+      <c t="n" r="L17" s="16">
         <v>10.5</v>
       </c>
-      <c t="n" s="17" r="M17">
+      <c t="n" r="M17" s="17">
         <v>10.15</v>
       </c>
     </row>
-    <row spans="1:13" r="18">
+    <row r="18" spans="1:13">
       <c t="n" r="A18">
         <v>2006</v>
       </c>
-      <c t="n" s="18" r="B18">
+      <c t="n" r="B18" s="18">
         <v>10.81</v>
       </c>
-      <c t="n" s="18" r="C18">
+      <c t="n" r="C18" s="18">
         <v>11.13</v>
       </c>
-      <c t="n" s="16" r="D18">
+      <c t="n" r="D18" s="16">
         <v>10.53</v>
       </c>
-      <c t="n" s="18" r="E18">
+      <c t="n" r="E18" s="18">
         <v>11.02</v>
       </c>
-      <c t="n" s="14" r="F18">
+      <c t="n" r="F18" s="14">
         <v>11.18</v>
       </c>
-      <c t="n" s="13" r="G18">
+      <c t="n" r="G18" s="13">
         <v>12.74</v>
       </c>
-      <c t="n" s="13" r="H18">
+      <c t="n" r="H18" s="13">
         <v>12.74</v>
       </c>
-      <c t="n" s="19" r="I18">
+      <c t="n" r="I18" s="19">
         <v>11.57</v>
       </c>
-      <c t="n" s="16" r="J18">
+      <c t="n" r="J18" s="16">
         <v>10.74</v>
       </c>
-      <c t="n" s="16" r="K18">
+      <c t="n" r="K18" s="16">
         <v>10.44</v>
       </c>
-      <c t="n" s="20" r="L18">
+      <c t="n" r="L18" s="20">
         <v>9.81</v>
       </c>
-      <c t="n" s="20" r="M18">
+      <c t="n" r="M18" s="20">
         <v>9.390000000000001</v>
       </c>
     </row>
-    <row spans="1:13" r="19">
+    <row r="19" spans="1:13">
       <c t="n" r="A19">
         <v>2007</v>
       </c>
-      <c t="n" s="20" r="B19">
+      <c t="n" r="B19" s="20">
         <v>9.869999999999999</v>
       </c>
-      <c t="n" s="20" r="C19">
+      <c t="n" r="C19" s="20">
         <v>9.699999999999999</v>
       </c>
-      <c t="n" s="14" r="D19">
+      <c t="n" r="D19" s="14">
         <v>11.21</v>
       </c>
-      <c t="n" s="14" r="E19">
+      <c t="n" r="E19" s="14">
         <v>11.46</v>
       </c>
-      <c t="n" s="21" r="F19">
+      <c t="n" r="F19" s="21">
         <v>12.08</v>
       </c>
-      <c t="n" s="15" r="G19">
+      <c t="n" r="G19" s="15">
         <v>12.43</v>
       </c>
-      <c t="n" s="9" r="H19">
+      <c t="n" r="H19" s="9">
         <v>14.62</v>
       </c>
-      <c t="n" s="3" r="I19">
+      <c t="n" r="I19" s="3">
         <v>19.33</v>
       </c>
-      <c t="n" s="31" r="J19">
+      <c t="n" r="J19" s="31">
         <v>16.91</v>
       </c>
-      <c t="n" s="28" r="K19">
+      <c t="n" r="K19" s="28">
         <v>16.08</v>
       </c>
-      <c t="n" s="4" r="L19">
+      <c t="n" r="L19" s="4">
         <v>17.38</v>
       </c>
-      <c t="n" s="25" r="M19">
+      <c t="n" r="M19" s="25">
         <v>18.28</v>
       </c>
     </row>
-    <row spans="1:13" r="20">
+    <row r="20" spans="1:13">
       <c t="n" r="A20">
         <v>2008</v>
       </c>
-      <c t="n" s="2" r="B20">
+      <c t="n" r="B20" s="2">
         <v>21.79</v>
       </c>
-      <c t="n" s="2" r="C20">
+      <c t="n" r="C20" s="2">
         <v>21.64</v>
       </c>
-      <c t="n" s="32" r="D20">
+      <c t="n" r="D20" s="32">
         <v>23.3</v>
       </c>
-      <c t="n" s="3" r="E20">
+      <c t="n" r="E20" s="3">
         <v>19.21</v>
       </c>
-      <c t="n" s="5" r="F20">
+      <c t="n" r="F20" s="5">
         <v>15.82</v>
       </c>
-      <c t="n" s="4" r="G20">
+      <c t="n" r="G20" s="4">
         <v>17.56</v>
       </c>
-      <c t="n" s="3" r="H20">
+      <c t="n" r="H20" s="3">
         <v>19.65</v>
       </c>
-      <c t="n" s="25" r="I20">
+      <c t="n" r="I20" s="25">
         <v>18.64</v>
       </c>
-      <c t="n" s="3" r="J20">
+      <c t="n" r="J20" s="3">
         <v>19.43</v>
       </c>
-      <c t="n" s="7" r="K20">
+      <c t="n" r="K20" s="7">
         <v>39.39</v>
       </c>
-      <c t="n" s="7" r="L20">
+      <c t="n" r="L20" s="7">
         <v>44.25</v>
       </c>
-      <c t="n" s="7" r="M20">
+      <c t="n" r="M20" s="7">
         <v>37.96</v>
       </c>
     </row>
-    <row spans="1:13" r="21">
+    <row r="21" spans="1:13">
       <c t="n" r="A21">
         <v>2009</v>
       </c>
-      <c t="n" s="7" r="B21">
+      <c t="n" r="B21" s="7">
         <v>33.76</v>
       </c>
-      <c t="n" s="7" r="C21">
+      <c t="n" r="C21" s="7">
         <v>40.73</v>
       </c>
-      <c t="n" s="7" r="D21">
+      <c t="n" r="D21" s="7">
         <v>38.79</v>
       </c>
-      <c t="n" s="7" r="E21">
+      <c t="n" r="E21" s="7">
         <v>33.68</v>
       </c>
-      <c t="n" s="8" r="F21">
+      <c t="n" r="F21" s="8">
         <v>26.57</v>
       </c>
-      <c t="n" s="29" r="G21">
+      <c t="n" r="G21" s="29">
         <v>25.02</v>
       </c>
-      <c t="n" s="32" r="H21">
+      <c t="n" r="H21" s="32">
         <v>23</v>
       </c>
-      <c t="n" s="32" r="I21">
+      <c t="n" r="I21" s="32">
         <v>22.58</v>
       </c>
-      <c t="n" s="2" r="J21">
+      <c t="n" r="J21" s="2">
         <v>22.19</v>
       </c>
-      <c t="n" s="27" r="K21">
+      <c t="n" r="K21" s="27">
         <v>20.1</v>
       </c>
-      <c t="n" s="27" r="L21">
+      <c t="n" r="L21" s="27">
         <v>20.05</v>
       </c>
-      <c t="n" s="3" r="M21">
+      <c t="n" r="M21" s="3">
         <v>19.25</v>
       </c>
     </row>
-    <row spans="1:13" r="22">
+    <row r="22" spans="1:13">
       <c t="n" r="A22">
         <v>2010</v>
       </c>
-      <c t="n" s="31" r="B22">
+      <c t="n" r="B22" s="31">
         <v>16.86</v>
       </c>
-      <c t="n" s="3" r="C22">
+      <c t="n" r="C22" s="3">
         <v>19.32</v>
       </c>
-      <c t="n" s="28" r="D22">
+      <c t="n" r="D22" s="28">
         <v>16.17</v>
       </c>
-      <c t="n" s="10" r="E22">
+      <c t="n" r="E22" s="10">
         <v>15.23</v>
       </c>
-      <c t="n" s="25" r="F22">
+      <c t="n" r="F22" s="25">
         <v>18.41</v>
       </c>
-      <c t="n" s="32" r="G22">
+      <c t="n" r="G22" s="32">
         <v>22.87</v>
       </c>
-      <c t="n" s="2" r="H22">
+      <c t="n" r="H22" s="2">
         <v>21.86</v>
       </c>
-      <c t="n" s="6" r="I22">
+      <c t="n" r="I22" s="6">
         <v>21.36</v>
       </c>
-      <c t="n" s="6" r="J22">
+      <c t="n" r="J22" s="6">
         <v>20.85</v>
       </c>
-      <c t="n" s="26" r="K22">
+      <c t="n" r="K22" s="26">
         <v>17.9</v>
       </c>
-      <c t="n" s="26" r="L22">
+      <c t="n" r="L22" s="26">
         <v>17.76</v>
       </c>
-      <c t="n" s="10" r="M22">
+      <c t="n" r="M22" s="10">
         <v>15.4</v>
       </c>
     </row>
-    <row spans="1:13" r="23">
+    <row r="23" spans="1:13">
       <c t="n" r="A23">
         <v>2011</v>
       </c>
-      <c t="n" s="10" r="B23">
+      <c t="n" r="B23" s="10">
         <v>15.37</v>
       </c>
-      <c t="n" s="9" r="C23">
+      <c t="n" r="C23" s="9">
         <v>14.86</v>
       </c>
-      <c t="n" s="31" r="D23">
+      <c t="n" r="D23" s="31">
         <v>17.07</v>
       </c>
-      <c t="n" s="11" r="E23">
+      <c t="n" r="E23" s="11">
         <v>14.27</v>
       </c>
-      <c t="n" s="11" r="F23">
+      <c t="n" r="F23" s="11">
         <v>14.49</v>
       </c>
-      <c t="n" s="28" r="G23">
+      <c t="n" r="G23" s="28">
         <v>15.88</v>
       </c>
-      <c t="n" s="10" r="H23">
+      <c t="n" r="H23" s="10">
         <v>15.12</v>
       </c>
-      <c t="n" s="2" r="I23">
+      <c t="n" r="I23" s="2">
         <v>22.46</v>
       </c>
-      <c t="n" s="7" r="J23">
+      <c t="n" r="J23" s="7">
         <v>30.43</v>
       </c>
-      <c t="n" s="29" r="K23">
+      <c t="n" r="K23" s="29">
         <v>24.44</v>
       </c>
-      <c t="n" s="8" r="L23">
+      <c t="n" r="L23" s="8">
         <v>27.03</v>
       </c>
-      <c t="n" s="27" r="M23">
+      <c t="n" r="M23" s="27">
         <v>20.34</v>
       </c>
     </row>
-    <row spans="1:13" r="24">
+    <row r="24" spans="1:13">
       <c t="n" r="A24">
         <v>2012</v>
       </c>
-      <c t="n" s="31" r="B24">
+      <c t="n" r="B24" s="31">
         <v>16.8</v>
       </c>
-      <c t="n" s="28" r="C24">
+      <c t="n" r="C24" s="28">
         <v>16.1</v>
       </c>
-      <c t="n" s="22" r="D24">
+      <c t="n" r="D24" s="22">
         <v>13.66</v>
       </c>
-      <c t="n" s="9" r="E24">
+      <c t="n" r="E24" s="9">
         <v>14.67</v>
       </c>
-      <c t="n" s="28" r="F24">
+      <c t="n" r="F24" s="28">
         <v>16.01</v>
       </c>
-      <c t="n" s="31" r="G24">
+      <c t="n" r="G24" s="31">
         <v>16.77</v>
       </c>
-      <c t="n" s="5" r="H24">
+      <c t="n" r="H24" s="5">
         <v>15.45</v>
       </c>
-      <c t="n" s="23" r="I24">
+      <c t="n" r="I24" s="23">
         <v>13.3</v>
       </c>
-      <c t="n" s="22" r="J24">
+      <c t="n" r="J24" s="22">
         <v>13.51</v>
       </c>
-      <c t="n" s="22" r="K24">
+      <c t="n" r="K24" s="22">
         <v>13.67</v>
       </c>
-      <c t="n" s="9" r="L24">
+      <c t="n" r="L24" s="9">
         <v>14.77</v>
       </c>
-      <c t="n" s="9" r="M24">
+      <c t="n" r="M24" s="9">
         <v>14.89</v>
       </c>
     </row>
-    <row spans="1:13" r="25">
+    <row r="25" spans="1:13">
       <c t="n" r="A25">
         <v>2013</v>
       </c>
-      <c t="n" s="21" r="B25">
+      <c t="n" r="B25" s="21">
         <v>12.29</v>
       </c>
-      <c t="n" s="21" r="C25">
+      <c t="n" r="C25" s="21">
         <v>12.08</v>
       </c>
-      <c t="n" s="18" r="D25">
+      <c t="n" r="D25" s="18">
         <v>11.05</v>
       </c>
-      <c t="n" s="21" r="E25">
+      <c t="n" r="E25" s="21">
         <v>11.99</v>
       </c>
-      <c t="n" s="21" r="F25">
+      <c t="n" r="F25" s="21">
         <v>12.26</v>
       </c>
-      <c t="n" s="11" r="G25">
+      <c t="n" r="G25" s="11">
         <v>14.36</v>
       </c>
-      <c t="n" s="21" r="H25">
+      <c t="n" r="H25" s="21">
         <v>12.07</v>
       </c>
-      <c t="n" s="19" r="I25">
+      <c t="n" r="I25" s="19">
         <v>11.83</v>
       </c>
-      <c t="n" s="15" r="J25">
+      <c t="n" r="J25" s="15">
         <v>12.52</v>
       </c>
-      <c t="n" s="15" r="K25">
+      <c t="n" r="K25" s="15">
         <v>12.34</v>
       </c>
-      <c t="n" s="21" r="L25">
+      <c t="n" r="L25" s="21">
         <v>11.99</v>
       </c>
-      <c t="n" s="19" r="M25">
+      <c t="n" r="M25" s="19">
         <v>11.69</v>
       </c>
     </row>
-    <row spans="1:13" r="26">
+    <row r="26" spans="1:13">
       <c t="n" r="A26">
         <v>2014</v>
       </c>
-      <c t="n" s="19" r="B26">
+      <c t="n" r="B26" s="19">
         <v>11.81</v>
       </c>
-      <c t="n" s="23" r="C26">
+      <c t="n" r="C26" s="23">
         <v>13.44</v>
       </c>
-      <c t="n" s="23" r="D26">
+      <c t="n" r="D26" s="23">
         <v>13.46</v>
       </c>
-      <c t="n" s="15" r="E26">
+      <c t="n" r="E26" s="15">
         <v>12.6</v>
       </c>
-      <c t="n" s="14" r="F26">
+      <c t="n" r="F26" s="14">
         <v>11.32</v>
       </c>
-      <c t="n" s="17" r="G26">
+      <c t="n" r="G26" s="17">
         <v>10.34</v>
       </c>
-      <c t="n" s="17" r="H26">
+      <c t="n" r="H26" s="17">
         <v>10.28</v>
       </c>
-      <c t="n" s="14" r="I26">
+      <c t="n" r="I26" s="14">
         <v>11.24</v>
       </c>
-      <c t="n" s="14" r="J26">
+      <c t="n" r="J26" s="14">
         <v>11.52</v>
       </c>
-      <c t="n" s="22" r="K26">
+      <c t="n" r="K26" s="22">
         <v>13.72</v>
       </c>
-      <c t="n" s="19" r="L26">
+      <c t="n" r="L26" s="19">
         <v>11.91</v>
       </c>
-      <c t="n" s="14" r="M26">
+      <c t="n" r="M26" s="14">
         <v>11.53</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" footer="0.5" header="0.5" bottom="1" left="0.75" right="0.75"/>
+  <pageMargins right="0.75" top="1" left="0.75" header="0.5" bottom="1" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>